<commit_message>
grid visualisation and power plant matching
</commit_message>
<xml_diff>
--- a/grid/substations.xlsx
+++ b/grid/substations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balazs.riskutia\FBMC\grid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balaz\SoftwareDeveloping\TUD\thesis\FBMC\grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D43F45-5A85-4EBE-9883-3612C6178B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE1D518-BC53-45C1-A511-ADD1E17445EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="21260" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4496" uniqueCount="1528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4529" uniqueCount="1540">
   <si>
     <t>name</t>
   </si>
@@ -3685,9 +3685,6 @@
     <t>KATOWICE</t>
   </si>
   <si>
-    <t xml:space="preserve">SCHIFFLANGE </t>
-  </si>
-  <si>
     <t>Grafenrheinfeld</t>
   </si>
   <si>
@@ -4604,6 +4601,45 @@
   </si>
   <si>
     <t>Wien</t>
+  </si>
+  <si>
+    <t>repiquage bifferdange 220kv</t>
+  </si>
+  <si>
+    <t>meiningen</t>
+  </si>
+  <si>
+    <t>walgauwerk</t>
+  </si>
+  <si>
+    <t>monceau</t>
+  </si>
+  <si>
+    <t>mt-saint-martin</t>
+  </si>
+  <si>
+    <t>sanem</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>sotel</t>
+  </si>
+  <si>
+    <t>vill</t>
+  </si>
+  <si>
+    <t>kempten</t>
+  </si>
+  <si>
+    <t>walgau</t>
+  </si>
+  <si>
+    <t>liskowiec</t>
+  </si>
+  <si>
+    <t>SCHIFFLANGE</t>
   </si>
 </sst>
 </file>
@@ -4632,7 +4668,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4655,15 +4691,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4966,10 +5012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1498"/>
+  <dimension ref="A1:F1509"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A622" workbookViewId="0">
-      <selection activeCell="B645" sqref="B645"/>
+    <sheetView tabSelected="1" topLeftCell="A1183" workbookViewId="0">
+      <selection activeCell="H1191" sqref="H1191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15036,7 +15082,7 @@
         <v>502</v>
       </c>
       <c r="B504" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="C504" t="s">
         <v>46</v>
@@ -17818,7 +17864,7 @@
         <v>642</v>
       </c>
       <c r="B644" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="C644" t="s">
         <v>68</v>
@@ -28766,7 +28812,7 @@
         <v>1190</v>
       </c>
       <c r="B1192" t="s">
-        <v>1221</v>
+        <v>1539</v>
       </c>
       <c r="C1192" t="s">
         <v>14</v>
@@ -28786,7 +28832,7 @@
         <v>1191</v>
       </c>
       <c r="B1193" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C1193" t="s">
         <v>14</v>
@@ -28806,7 +28852,7 @@
         <v>1192</v>
       </c>
       <c r="B1194" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C1194" t="s">
         <v>24</v>
@@ -28826,7 +28872,7 @@
         <v>1193</v>
       </c>
       <c r="B1195" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C1195" t="s">
         <v>9</v>
@@ -28846,7 +28892,7 @@
         <v>1194</v>
       </c>
       <c r="B1196" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C1196" t="s">
         <v>9</v>
@@ -28866,7 +28912,7 @@
         <v>1195</v>
       </c>
       <c r="B1197" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C1197" t="s">
         <v>14</v>
@@ -28886,7 +28932,7 @@
         <v>1196</v>
       </c>
       <c r="B1198" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C1198" t="s">
         <v>9</v>
@@ -28906,7 +28952,7 @@
         <v>1197</v>
       </c>
       <c r="B1199" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C1199" t="s">
         <v>77</v>
@@ -28926,7 +28972,7 @@
         <v>1198</v>
       </c>
       <c r="B1200" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C1200" t="s">
         <v>38</v>
@@ -28946,7 +28992,7 @@
         <v>1199</v>
       </c>
       <c r="B1201" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="C1201" t="s">
         <v>9</v>
@@ -28966,7 +29012,7 @@
         <v>1200</v>
       </c>
       <c r="B1202" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C1202" t="s">
         <v>24</v>
@@ -28986,7 +29032,7 @@
         <v>1201</v>
       </c>
       <c r="B1203" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C1203" t="s">
         <v>9</v>
@@ -29006,7 +29052,7 @@
         <v>1202</v>
       </c>
       <c r="B1204" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C1204" t="s">
         <v>14</v>
@@ -29026,7 +29072,7 @@
         <v>1203</v>
       </c>
       <c r="B1205" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C1205" t="s">
         <v>24</v>
@@ -29046,7 +29092,7 @@
         <v>1204</v>
       </c>
       <c r="B1206" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C1206" t="s">
         <v>14</v>
@@ -29066,7 +29112,7 @@
         <v>1205</v>
       </c>
       <c r="B1207" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C1207" t="s">
         <v>9</v>
@@ -29086,7 +29132,7 @@
         <v>1206</v>
       </c>
       <c r="B1208" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C1208" t="s">
         <v>9</v>
@@ -29106,7 +29152,7 @@
         <v>1207</v>
       </c>
       <c r="B1209" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C1209" t="s">
         <v>14</v>
@@ -29126,7 +29172,7 @@
         <v>1208</v>
       </c>
       <c r="B1210" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C1210" t="s">
         <v>14</v>
@@ -29146,7 +29192,7 @@
         <v>1209</v>
       </c>
       <c r="B1211" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="C1211" t="s">
         <v>9</v>
@@ -29166,7 +29212,7 @@
         <v>1210</v>
       </c>
       <c r="B1212" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C1212" t="s">
         <v>14</v>
@@ -29186,7 +29232,7 @@
         <v>1211</v>
       </c>
       <c r="B1213" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C1213" t="s">
         <v>24</v>
@@ -29206,7 +29252,7 @@
         <v>1212</v>
       </c>
       <c r="B1214" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C1214" t="s">
         <v>9</v>
@@ -29226,7 +29272,7 @@
         <v>1213</v>
       </c>
       <c r="B1215" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C1215" t="s">
         <v>9</v>
@@ -29246,7 +29292,7 @@
         <v>1214</v>
       </c>
       <c r="B1216" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C1216" t="s">
         <v>14</v>
@@ -29266,7 +29312,7 @@
         <v>1215</v>
       </c>
       <c r="B1217" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C1217" t="s">
         <v>9</v>
@@ -29286,7 +29332,7 @@
         <v>1216</v>
       </c>
       <c r="B1218" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C1218" t="s">
         <v>14</v>
@@ -29306,7 +29352,7 @@
         <v>1217</v>
       </c>
       <c r="B1219" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="C1219" t="s">
         <v>9</v>
@@ -29326,7 +29372,7 @@
         <v>1218</v>
       </c>
       <c r="B1220" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C1220" t="s">
         <v>24</v>
@@ -29346,7 +29392,7 @@
         <v>1219</v>
       </c>
       <c r="B1221" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C1221" t="s">
         <v>9</v>
@@ -29366,7 +29412,7 @@
         <v>1220</v>
       </c>
       <c r="B1222" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C1222" t="s">
         <v>14</v>
@@ -29386,7 +29432,7 @@
         <v>1221</v>
       </c>
       <c r="B1223" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C1223" t="s">
         <v>77</v>
@@ -29406,7 +29452,7 @@
         <v>1222</v>
       </c>
       <c r="B1224" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="C1224" t="s">
         <v>9</v>
@@ -29426,7 +29472,7 @@
         <v>1223</v>
       </c>
       <c r="B1225" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="C1225" t="s">
         <v>14</v>
@@ -29446,7 +29492,7 @@
         <v>1224</v>
       </c>
       <c r="B1226" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C1226" t="s">
         <v>14</v>
@@ -29466,7 +29512,7 @@
         <v>1225</v>
       </c>
       <c r="B1227" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C1227" t="s">
         <v>9</v>
@@ -29486,7 +29532,7 @@
         <v>1226</v>
       </c>
       <c r="B1228" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="C1228" t="s">
         <v>14</v>
@@ -29506,7 +29552,7 @@
         <v>1227</v>
       </c>
       <c r="B1229" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="C1229" t="s">
         <v>14</v>
@@ -29546,7 +29592,7 @@
         <v>1229</v>
       </c>
       <c r="B1231" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C1231" t="s">
         <v>14</v>
@@ -29566,7 +29612,7 @@
         <v>1230</v>
       </c>
       <c r="B1232" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C1232" t="s">
         <v>9</v>
@@ -29586,7 +29632,7 @@
         <v>1231</v>
       </c>
       <c r="B1233" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C1233" t="s">
         <v>6</v>
@@ -29606,7 +29652,7 @@
         <v>1232</v>
       </c>
       <c r="B1234" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C1234" t="s">
         <v>14</v>
@@ -29626,7 +29672,7 @@
         <v>1233</v>
       </c>
       <c r="B1235" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C1235" t="s">
         <v>9</v>
@@ -29646,7 +29692,7 @@
         <v>1234</v>
       </c>
       <c r="B1236" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C1236" t="s">
         <v>9</v>
@@ -29666,7 +29712,7 @@
         <v>1235</v>
       </c>
       <c r="B1237" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C1237" t="s">
         <v>24</v>
@@ -29686,7 +29732,7 @@
         <v>1236</v>
       </c>
       <c r="B1238" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C1238" t="s">
         <v>77</v>
@@ -29706,7 +29752,7 @@
         <v>1237</v>
       </c>
       <c r="B1239" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C1239" t="s">
         <v>9</v>
@@ -29726,7 +29772,7 @@
         <v>1238</v>
       </c>
       <c r="B1240" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C1240" t="s">
         <v>9</v>
@@ -29746,7 +29792,7 @@
         <v>1239</v>
       </c>
       <c r="B1241" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C1241" t="s">
         <v>14</v>
@@ -29766,7 +29812,7 @@
         <v>1240</v>
       </c>
       <c r="B1242" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C1242" t="s">
         <v>38</v>
@@ -29786,7 +29832,7 @@
         <v>1241</v>
       </c>
       <c r="B1243" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C1243" t="s">
         <v>9</v>
@@ -29806,7 +29852,7 @@
         <v>1242</v>
       </c>
       <c r="B1244" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C1244" t="s">
         <v>64</v>
@@ -29826,7 +29872,7 @@
         <v>1243</v>
       </c>
       <c r="B1245" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C1245" t="s">
         <v>24</v>
@@ -29846,7 +29892,7 @@
         <v>1244</v>
       </c>
       <c r="B1246" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C1246" t="s">
         <v>9</v>
@@ -29866,7 +29912,7 @@
         <v>1245</v>
       </c>
       <c r="B1247" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C1247" t="s">
         <v>387</v>
@@ -29886,7 +29932,7 @@
         <v>1246</v>
       </c>
       <c r="B1248" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C1248" t="s">
         <v>14</v>
@@ -29906,7 +29952,7 @@
         <v>1247</v>
       </c>
       <c r="B1249" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C1249" t="s">
         <v>14</v>
@@ -29926,7 +29972,7 @@
         <v>1248</v>
       </c>
       <c r="B1250" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C1250" t="s">
         <v>9</v>
@@ -29946,7 +29992,7 @@
         <v>1249</v>
       </c>
       <c r="B1251" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="C1251" t="s">
         <v>38</v>
@@ -29966,7 +30012,7 @@
         <v>1250</v>
       </c>
       <c r="B1252" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C1252" t="s">
         <v>6</v>
@@ -29986,7 +30032,7 @@
         <v>1251</v>
       </c>
       <c r="B1253" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C1253" t="s">
         <v>14</v>
@@ -30006,7 +30052,7 @@
         <v>1252</v>
       </c>
       <c r="B1254" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C1254" t="s">
         <v>24</v>
@@ -30026,7 +30072,7 @@
         <v>1253</v>
       </c>
       <c r="B1255" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="C1255" t="s">
         <v>9</v>
@@ -30046,7 +30092,7 @@
         <v>1254</v>
       </c>
       <c r="B1256" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C1256" t="s">
         <v>38</v>
@@ -30066,7 +30112,7 @@
         <v>1255</v>
       </c>
       <c r="B1257" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="C1257" t="s">
         <v>14</v>
@@ -30086,7 +30132,7 @@
         <v>1256</v>
       </c>
       <c r="B1258" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C1258" t="s">
         <v>14</v>
@@ -30106,7 +30152,7 @@
         <v>1257</v>
       </c>
       <c r="B1259" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="C1259" t="s">
         <v>38</v>
@@ -30126,7 +30172,7 @@
         <v>1258</v>
       </c>
       <c r="B1260" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C1260" t="s">
         <v>14</v>
@@ -30146,7 +30192,7 @@
         <v>1259</v>
       </c>
       <c r="B1261" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C1261" t="s">
         <v>9</v>
@@ -30166,7 +30212,7 @@
         <v>1260</v>
       </c>
       <c r="B1262" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C1262" t="s">
         <v>14</v>
@@ -30186,7 +30232,7 @@
         <v>1261</v>
       </c>
       <c r="B1263" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1263" t="s">
         <v>14</v>
@@ -30206,7 +30252,7 @@
         <v>1262</v>
       </c>
       <c r="B1264" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C1264" t="s">
         <v>14</v>
@@ -30226,7 +30272,7 @@
         <v>1263</v>
       </c>
       <c r="B1265" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C1265" t="s">
         <v>9</v>
@@ -30246,7 +30292,7 @@
         <v>1264</v>
       </c>
       <c r="B1266" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C1266" t="s">
         <v>14</v>
@@ -30266,7 +30312,7 @@
         <v>1265</v>
       </c>
       <c r="B1267" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C1267" t="s">
         <v>20</v>
@@ -30286,7 +30332,7 @@
         <v>1266</v>
       </c>
       <c r="B1268" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C1268" t="s">
         <v>6</v>
@@ -30306,7 +30352,7 @@
         <v>1267</v>
       </c>
       <c r="B1269" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C1269" t="s">
         <v>9</v>
@@ -30326,7 +30372,7 @@
         <v>1268</v>
       </c>
       <c r="B1270" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C1270" t="s">
         <v>9</v>
@@ -30346,7 +30392,7 @@
         <v>1269</v>
       </c>
       <c r="B1271" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C1271" t="s">
         <v>38</v>
@@ -30366,7 +30412,7 @@
         <v>1270</v>
       </c>
       <c r="B1272" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C1272" t="s">
         <v>6</v>
@@ -30386,7 +30432,7 @@
         <v>1271</v>
       </c>
       <c r="B1273" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="C1273" t="s">
         <v>9</v>
@@ -30400,7 +30446,7 @@
         <v>1272</v>
       </c>
       <c r="B1274" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C1274" t="s">
         <v>9</v>
@@ -30420,7 +30466,7 @@
         <v>1273</v>
       </c>
       <c r="B1275" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="C1275" t="s">
         <v>14</v>
@@ -30440,7 +30486,7 @@
         <v>1274</v>
       </c>
       <c r="B1276" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C1276" t="s">
         <v>9</v>
@@ -30460,7 +30506,7 @@
         <v>1275</v>
       </c>
       <c r="B1277" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C1277" t="s">
         <v>9</v>
@@ -30480,7 +30526,7 @@
         <v>1276</v>
       </c>
       <c r="B1278" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C1278" t="s">
         <v>14</v>
@@ -30500,7 +30546,7 @@
         <v>1277</v>
       </c>
       <c r="B1279" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C1279" t="s">
         <v>9</v>
@@ -30520,7 +30566,7 @@
         <v>1278</v>
       </c>
       <c r="B1280" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C1280" t="s">
         <v>9</v>
@@ -30540,7 +30586,7 @@
         <v>1279</v>
       </c>
       <c r="B1281" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C1281" t="s">
         <v>14</v>
@@ -30560,7 +30606,7 @@
         <v>1280</v>
       </c>
       <c r="B1282" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C1282" t="s">
         <v>68</v>
@@ -30580,7 +30626,7 @@
         <v>1281</v>
       </c>
       <c r="B1283" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1283" t="s">
         <v>9</v>
@@ -30600,7 +30646,7 @@
         <v>1282</v>
       </c>
       <c r="B1284" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C1284" t="s">
         <v>38</v>
@@ -30620,7 +30666,7 @@
         <v>1283</v>
       </c>
       <c r="B1285" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C1285" t="s">
         <v>24</v>
@@ -30640,7 +30686,7 @@
         <v>1284</v>
       </c>
       <c r="B1286" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C1286" t="s">
         <v>9</v>
@@ -30660,7 +30706,7 @@
         <v>1285</v>
       </c>
       <c r="B1287" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="C1287" t="s">
         <v>9</v>
@@ -30680,7 +30726,7 @@
         <v>1286</v>
       </c>
       <c r="B1288" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C1288" t="s">
         <v>9</v>
@@ -30700,7 +30746,7 @@
         <v>1287</v>
       </c>
       <c r="B1289" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="C1289" t="s">
         <v>24</v>
@@ -30720,7 +30766,7 @@
         <v>1288</v>
       </c>
       <c r="B1290" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C1290" t="s">
         <v>14</v>
@@ -30740,7 +30786,7 @@
         <v>1289</v>
       </c>
       <c r="B1291" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C1291" t="s">
         <v>14</v>
@@ -30760,7 +30806,7 @@
         <v>1290</v>
       </c>
       <c r="B1292" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C1292" t="s">
         <v>14</v>
@@ -30780,7 +30826,7 @@
         <v>1291</v>
       </c>
       <c r="B1293" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C1293" t="s">
         <v>24</v>
@@ -30800,7 +30846,7 @@
         <v>1292</v>
       </c>
       <c r="B1294" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="C1294" t="s">
         <v>9</v>
@@ -30820,7 +30866,7 @@
         <v>1293</v>
       </c>
       <c r="B1295" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C1295" t="s">
         <v>14</v>
@@ -30840,7 +30886,7 @@
         <v>1294</v>
       </c>
       <c r="B1296" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C1296" t="s">
         <v>14</v>
@@ -30860,7 +30906,7 @@
         <v>1295</v>
       </c>
       <c r="B1297" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C1297" t="s">
         <v>14</v>
@@ -30880,7 +30926,7 @@
         <v>1296</v>
       </c>
       <c r="B1298" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="C1298" t="s">
         <v>6</v>
@@ -30900,7 +30946,7 @@
         <v>1297</v>
       </c>
       <c r="B1299" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="C1299" t="s">
         <v>14</v>
@@ -30920,7 +30966,7 @@
         <v>1298</v>
       </c>
       <c r="B1300" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="C1300" t="s">
         <v>9</v>
@@ -30940,7 +30986,7 @@
         <v>1299</v>
       </c>
       <c r="B1301" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="C1301" t="s">
         <v>14</v>
@@ -30960,7 +31006,7 @@
         <v>1300</v>
       </c>
       <c r="B1302" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="C1302" t="s">
         <v>14</v>
@@ -30980,7 +31026,7 @@
         <v>1301</v>
       </c>
       <c r="B1303" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="C1303" t="s">
         <v>14</v>
@@ -31000,7 +31046,7 @@
         <v>1302</v>
       </c>
       <c r="B1304" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="C1304" t="s">
         <v>9</v>
@@ -31020,7 +31066,7 @@
         <v>1303</v>
       </c>
       <c r="B1305" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C1305" t="s">
         <v>6</v>
@@ -31040,7 +31086,7 @@
         <v>1304</v>
       </c>
       <c r="B1306" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C1306" t="s">
         <v>14</v>
@@ -31060,7 +31106,7 @@
         <v>1305</v>
       </c>
       <c r="B1307" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C1307" t="s">
         <v>9</v>
@@ -31080,7 +31126,7 @@
         <v>1306</v>
       </c>
       <c r="B1308" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C1308" t="s">
         <v>9</v>
@@ -31100,7 +31146,7 @@
         <v>1307</v>
       </c>
       <c r="B1309" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="C1309" t="s">
         <v>24</v>
@@ -31120,7 +31166,7 @@
         <v>1308</v>
       </c>
       <c r="B1310" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="C1310" t="s">
         <v>46</v>
@@ -31140,7 +31186,7 @@
         <v>1309</v>
       </c>
       <c r="B1311" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="C1311" t="s">
         <v>6</v>
@@ -31160,7 +31206,7 @@
         <v>1310</v>
       </c>
       <c r="B1312" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="C1312" t="s">
         <v>6</v>
@@ -31180,7 +31226,7 @@
         <v>1311</v>
       </c>
       <c r="B1313" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="C1313" t="s">
         <v>14</v>
@@ -31200,7 +31246,7 @@
         <v>1312</v>
       </c>
       <c r="B1314" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="C1314" t="s">
         <v>9</v>
@@ -31220,7 +31266,7 @@
         <v>1313</v>
       </c>
       <c r="B1315" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="C1315" t="s">
         <v>14</v>
@@ -31240,7 +31286,7 @@
         <v>1314</v>
       </c>
       <c r="B1316" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="C1316" t="s">
         <v>14</v>
@@ -31260,7 +31306,7 @@
         <v>1315</v>
       </c>
       <c r="B1317" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="C1317" t="s">
         <v>46</v>
@@ -31280,7 +31326,7 @@
         <v>1316</v>
       </c>
       <c r="B1318" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C1318" t="s">
         <v>9</v>
@@ -31300,7 +31346,7 @@
         <v>1317</v>
       </c>
       <c r="B1319" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="C1319" t="s">
         <v>6</v>
@@ -31320,7 +31366,7 @@
         <v>1318</v>
       </c>
       <c r="B1320" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C1320" t="s">
         <v>14</v>
@@ -31340,7 +31386,7 @@
         <v>1319</v>
       </c>
       <c r="B1321" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C1321" t="s">
         <v>9</v>
@@ -31360,7 +31406,7 @@
         <v>1320</v>
       </c>
       <c r="B1322" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C1322" t="s">
         <v>14</v>
@@ -31380,7 +31426,7 @@
         <v>1321</v>
       </c>
       <c r="B1323" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C1323" t="s">
         <v>9</v>
@@ -31400,7 +31446,7 @@
         <v>1322</v>
       </c>
       <c r="B1324" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C1324" t="s">
         <v>68</v>
@@ -31420,7 +31466,7 @@
         <v>1323</v>
       </c>
       <c r="B1325" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="C1325" t="s">
         <v>9</v>
@@ -31440,7 +31486,7 @@
         <v>1324</v>
       </c>
       <c r="B1326" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C1326" t="s">
         <v>68</v>
@@ -31460,7 +31506,7 @@
         <v>1325</v>
       </c>
       <c r="B1327" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C1327" t="s">
         <v>20</v>
@@ -31480,7 +31526,7 @@
         <v>1326</v>
       </c>
       <c r="B1328" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C1328" t="s">
         <v>9</v>
@@ -31500,7 +31546,7 @@
         <v>1327</v>
       </c>
       <c r="B1329" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C1329" t="s">
         <v>14</v>
@@ -31520,7 +31566,7 @@
         <v>1328</v>
       </c>
       <c r="B1330" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C1330" t="s">
         <v>9</v>
@@ -31540,7 +31586,7 @@
         <v>1329</v>
       </c>
       <c r="B1331" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C1331" t="s">
         <v>9</v>
@@ -31560,7 +31606,7 @@
         <v>1330</v>
       </c>
       <c r="B1332" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C1332" t="s">
         <v>14</v>
@@ -31580,7 +31626,7 @@
         <v>1331</v>
       </c>
       <c r="B1333" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="C1333" t="s">
         <v>9</v>
@@ -31600,7 +31646,7 @@
         <v>1332</v>
       </c>
       <c r="B1334" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="C1334" t="s">
         <v>9</v>
@@ -31620,7 +31666,7 @@
         <v>1333</v>
       </c>
       <c r="B1335" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C1335" t="s">
         <v>387</v>
@@ -31640,7 +31686,7 @@
         <v>1334</v>
       </c>
       <c r="B1336" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="C1336" t="s">
         <v>24</v>
@@ -31660,7 +31706,7 @@
         <v>1335</v>
       </c>
       <c r="B1337" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C1337" t="s">
         <v>14</v>
@@ -31680,7 +31726,7 @@
         <v>1336</v>
       </c>
       <c r="B1338" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C1338" t="s">
         <v>6</v>
@@ -31700,7 +31746,7 @@
         <v>1337</v>
       </c>
       <c r="B1339" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C1339" t="s">
         <v>24</v>
@@ -31720,7 +31766,7 @@
         <v>1338</v>
       </c>
       <c r="B1340" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="C1340" t="s">
         <v>6</v>
@@ -31740,7 +31786,7 @@
         <v>1339</v>
       </c>
       <c r="B1341" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="C1341" t="s">
         <v>14</v>
@@ -31760,7 +31806,7 @@
         <v>1340</v>
       </c>
       <c r="B1342" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="C1342" t="s">
         <v>9</v>
@@ -31780,7 +31826,7 @@
         <v>1341</v>
       </c>
       <c r="B1343" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="C1343" t="s">
         <v>9</v>
@@ -31800,7 +31846,7 @@
         <v>1342</v>
       </c>
       <c r="B1344" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="C1344" t="s">
         <v>14</v>
@@ -31820,7 +31866,7 @@
         <v>1343</v>
       </c>
       <c r="B1345" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="C1345" t="s">
         <v>64</v>
@@ -31840,7 +31886,7 @@
         <v>1344</v>
       </c>
       <c r="B1346" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="C1346" t="s">
         <v>14</v>
@@ -31860,7 +31906,7 @@
         <v>1345</v>
       </c>
       <c r="B1347" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="C1347" t="s">
         <v>14</v>
@@ -31880,7 +31926,7 @@
         <v>1346</v>
       </c>
       <c r="B1348" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="C1348" t="s">
         <v>9</v>
@@ -31900,7 +31946,7 @@
         <v>1347</v>
       </c>
       <c r="B1349" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="C1349" t="s">
         <v>9</v>
@@ -31920,7 +31966,7 @@
         <v>1348</v>
       </c>
       <c r="B1350" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="C1350" t="s">
         <v>9</v>
@@ -31940,7 +31986,7 @@
         <v>1349</v>
       </c>
       <c r="B1351" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="C1351" t="s">
         <v>9</v>
@@ -31960,7 +32006,7 @@
         <v>1350</v>
       </c>
       <c r="B1352" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="C1352" t="s">
         <v>14</v>
@@ -31980,7 +32026,7 @@
         <v>1351</v>
       </c>
       <c r="B1353" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C1353" t="s">
         <v>38</v>
@@ -32000,7 +32046,7 @@
         <v>1352</v>
       </c>
       <c r="B1354" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="C1354" t="s">
         <v>9</v>
@@ -32020,7 +32066,7 @@
         <v>1353</v>
       </c>
       <c r="B1355" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C1355" t="s">
         <v>68</v>
@@ -32040,7 +32086,7 @@
         <v>1354</v>
       </c>
       <c r="B1356" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="C1356" t="s">
         <v>77</v>
@@ -32060,7 +32106,7 @@
         <v>1355</v>
       </c>
       <c r="B1357" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="C1357" t="s">
         <v>6</v>
@@ -32080,7 +32126,7 @@
         <v>1356</v>
       </c>
       <c r="B1358" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C1358" t="s">
         <v>9</v>
@@ -32100,7 +32146,7 @@
         <v>1357</v>
       </c>
       <c r="B1359" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="C1359" t="s">
         <v>9</v>
@@ -32120,7 +32166,7 @@
         <v>1358</v>
       </c>
       <c r="B1360" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="C1360" t="s">
         <v>6</v>
@@ -32140,7 +32186,7 @@
         <v>1359</v>
       </c>
       <c r="B1361" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="C1361" t="s">
         <v>9</v>
@@ -32160,7 +32206,7 @@
         <v>1360</v>
       </c>
       <c r="B1362" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="C1362" t="s">
         <v>9</v>
@@ -32180,7 +32226,7 @@
         <v>1361</v>
       </c>
       <c r="B1363" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="C1363" t="s">
         <v>9</v>
@@ -32200,7 +32246,7 @@
         <v>1362</v>
       </c>
       <c r="B1364" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="C1364" t="s">
         <v>387</v>
@@ -32220,7 +32266,7 @@
         <v>1363</v>
       </c>
       <c r="B1365" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C1365" t="s">
         <v>64</v>
@@ -32240,7 +32286,7 @@
         <v>1364</v>
       </c>
       <c r="B1366" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="C1366" t="s">
         <v>14</v>
@@ -32260,7 +32306,7 @@
         <v>1365</v>
       </c>
       <c r="B1367" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="C1367" t="s">
         <v>9</v>
@@ -32280,7 +32326,7 @@
         <v>1366</v>
       </c>
       <c r="B1368" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="C1368" t="s">
         <v>9</v>
@@ -32300,7 +32346,7 @@
         <v>1367</v>
       </c>
       <c r="B1369" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="C1369" t="s">
         <v>14</v>
@@ -32320,7 +32366,7 @@
         <v>1368</v>
       </c>
       <c r="B1370" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="C1370" t="s">
         <v>14</v>
@@ -32340,7 +32386,7 @@
         <v>1369</v>
       </c>
       <c r="B1371" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="C1371" t="s">
         <v>64</v>
@@ -32360,7 +32406,7 @@
         <v>1370</v>
       </c>
       <c r="B1372" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="C1372" t="s">
         <v>14</v>
@@ -32380,7 +32426,7 @@
         <v>1371</v>
       </c>
       <c r="B1373" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="C1373" t="s">
         <v>6</v>
@@ -32400,7 +32446,7 @@
         <v>1372</v>
       </c>
       <c r="B1374" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="C1374" t="s">
         <v>9</v>
@@ -32420,7 +32466,7 @@
         <v>1373</v>
       </c>
       <c r="B1375" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="C1375" t="s">
         <v>9</v>
@@ -32440,7 +32486,7 @@
         <v>1374</v>
       </c>
       <c r="B1376" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="C1376" t="s">
         <v>14</v>
@@ -32460,7 +32506,7 @@
         <v>1375</v>
       </c>
       <c r="B1377" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="C1377" t="s">
         <v>9</v>
@@ -32480,7 +32526,7 @@
         <v>1376</v>
       </c>
       <c r="B1378" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="C1378" t="s">
         <v>68</v>
@@ -32500,7 +32546,7 @@
         <v>1377</v>
       </c>
       <c r="B1379" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="C1379" t="s">
         <v>68</v>
@@ -32520,7 +32566,7 @@
         <v>1378</v>
       </c>
       <c r="B1380" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="C1380" t="s">
         <v>46</v>
@@ -32540,7 +32586,7 @@
         <v>1379</v>
       </c>
       <c r="B1381" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="C1381" t="s">
         <v>9</v>
@@ -32560,7 +32606,7 @@
         <v>1380</v>
       </c>
       <c r="B1382" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="C1382" t="s">
         <v>6</v>
@@ -32580,7 +32626,7 @@
         <v>1381</v>
       </c>
       <c r="B1383" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="C1383" t="s">
         <v>64</v>
@@ -32600,7 +32646,7 @@
         <v>1382</v>
       </c>
       <c r="B1384" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="C1384" t="s">
         <v>9</v>
@@ -32620,7 +32666,7 @@
         <v>1383</v>
       </c>
       <c r="B1385" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="C1385" t="s">
         <v>9</v>
@@ -32640,7 +32686,7 @@
         <v>1384</v>
       </c>
       <c r="B1386" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C1386" t="s">
         <v>9</v>
@@ -32660,7 +32706,7 @@
         <v>1385</v>
       </c>
       <c r="B1387" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="C1387" t="s">
         <v>6</v>
@@ -32680,7 +32726,7 @@
         <v>1386</v>
       </c>
       <c r="B1388" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="C1388" t="s">
         <v>14</v>
@@ -32700,7 +32746,7 @@
         <v>1387</v>
       </c>
       <c r="B1389" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="C1389" t="s">
         <v>9</v>
@@ -32720,7 +32766,7 @@
         <v>1388</v>
       </c>
       <c r="B1390" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="C1390" t="s">
         <v>24</v>
@@ -32740,7 +32786,7 @@
         <v>1389</v>
       </c>
       <c r="B1391" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="C1391" t="s">
         <v>9</v>
@@ -32760,7 +32806,7 @@
         <v>1390</v>
       </c>
       <c r="B1392" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="C1392" t="s">
         <v>14</v>
@@ -32780,7 +32826,7 @@
         <v>1391</v>
       </c>
       <c r="B1393" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="C1393" t="s">
         <v>9</v>
@@ -32800,7 +32846,7 @@
         <v>1392</v>
       </c>
       <c r="B1394" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C1394" t="s">
         <v>34</v>
@@ -32820,7 +32866,7 @@
         <v>1393</v>
       </c>
       <c r="B1395" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="C1395" t="s">
         <v>14</v>
@@ -32840,7 +32886,7 @@
         <v>1394</v>
       </c>
       <c r="B1396" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C1396" t="s">
         <v>14</v>
@@ -32860,7 +32906,7 @@
         <v>1395</v>
       </c>
       <c r="B1397" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C1397" t="s">
         <v>6</v>
@@ -32880,7 +32926,7 @@
         <v>1396</v>
       </c>
       <c r="B1398" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="C1398" t="s">
         <v>14</v>
@@ -32900,7 +32946,7 @@
         <v>1397</v>
       </c>
       <c r="B1399" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="C1399" t="s">
         <v>38</v>
@@ -32920,7 +32966,7 @@
         <v>1398</v>
       </c>
       <c r="B1400" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="C1400" t="s">
         <v>14</v>
@@ -32940,7 +32986,7 @@
         <v>1399</v>
       </c>
       <c r="B1401" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="C1401" t="s">
         <v>38</v>
@@ -32960,7 +33006,7 @@
         <v>1400</v>
       </c>
       <c r="B1402" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="C1402" t="s">
         <v>9</v>
@@ -32980,7 +33026,7 @@
         <v>1401</v>
       </c>
       <c r="B1403" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="C1403" t="s">
         <v>9</v>
@@ -33000,7 +33046,7 @@
         <v>1402</v>
       </c>
       <c r="B1404" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="C1404" t="s">
         <v>38</v>
@@ -33020,7 +33066,7 @@
         <v>1403</v>
       </c>
       <c r="B1405" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="C1405" t="s">
         <v>14</v>
@@ -33040,7 +33086,7 @@
         <v>1404</v>
       </c>
       <c r="B1406" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="C1406" t="s">
         <v>46</v>
@@ -33060,7 +33106,7 @@
         <v>1405</v>
       </c>
       <c r="B1407" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="C1407" t="s">
         <v>9</v>
@@ -33080,7 +33126,7 @@
         <v>1406</v>
       </c>
       <c r="B1408" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C1408" t="s">
         <v>24</v>
@@ -33100,7 +33146,7 @@
         <v>1407</v>
       </c>
       <c r="B1409" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="C1409" t="s">
         <v>9</v>
@@ -33120,7 +33166,7 @@
         <v>1408</v>
       </c>
       <c r="B1410" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="C1410" t="s">
         <v>9</v>
@@ -33140,7 +33186,7 @@
         <v>1409</v>
       </c>
       <c r="B1411" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="C1411" t="s">
         <v>9</v>
@@ -33160,7 +33206,7 @@
         <v>1410</v>
       </c>
       <c r="B1412" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="C1412" t="s">
         <v>14</v>
@@ -33180,7 +33226,7 @@
         <v>1411</v>
       </c>
       <c r="B1413" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C1413" t="s">
         <v>34</v>
@@ -33200,7 +33246,7 @@
         <v>1412</v>
       </c>
       <c r="B1414" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="C1414" t="s">
         <v>9</v>
@@ -33220,7 +33266,7 @@
         <v>1413</v>
       </c>
       <c r="B1415" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="C1415" t="s">
         <v>14</v>
@@ -33240,7 +33286,7 @@
         <v>1414</v>
       </c>
       <c r="B1416" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="C1416" t="s">
         <v>64</v>
@@ -33260,7 +33306,7 @@
         <v>1415</v>
       </c>
       <c r="B1417" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="C1417" t="s">
         <v>9</v>
@@ -33280,7 +33326,7 @@
         <v>1416</v>
       </c>
       <c r="B1418" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="C1418" t="s">
         <v>9</v>
@@ -33300,7 +33346,7 @@
         <v>1417</v>
       </c>
       <c r="B1419" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="C1419" t="s">
         <v>6</v>
@@ -33320,7 +33366,7 @@
         <v>1418</v>
       </c>
       <c r="B1420" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="C1420" t="s">
         <v>14</v>
@@ -33340,7 +33386,7 @@
         <v>1419</v>
       </c>
       <c r="B1421" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="C1421" t="s">
         <v>6</v>
@@ -33360,7 +33406,7 @@
         <v>1420</v>
       </c>
       <c r="B1422" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="C1422" t="s">
         <v>64</v>
@@ -33380,7 +33426,7 @@
         <v>1421</v>
       </c>
       <c r="B1423" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C1423" t="s">
         <v>9</v>
@@ -33400,7 +33446,7 @@
         <v>1422</v>
       </c>
       <c r="B1424" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="C1424" t="s">
         <v>9</v>
@@ -33420,7 +33466,7 @@
         <v>1423</v>
       </c>
       <c r="B1425" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="C1425" t="s">
         <v>14</v>
@@ -33440,7 +33486,7 @@
         <v>1424</v>
       </c>
       <c r="B1426" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="C1426" t="s">
         <v>9</v>
@@ -33460,7 +33506,7 @@
         <v>1425</v>
       </c>
       <c r="B1427" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="C1427" t="s">
         <v>14</v>
@@ -33480,7 +33526,7 @@
         <v>1426</v>
       </c>
       <c r="B1428" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="C1428" t="s">
         <v>14</v>
@@ -33500,7 +33546,7 @@
         <v>1427</v>
       </c>
       <c r="B1429" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="C1429" t="s">
         <v>14</v>
@@ -33520,7 +33566,7 @@
         <v>1428</v>
       </c>
       <c r="B1430" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="C1430" t="s">
         <v>24</v>
@@ -33540,7 +33586,7 @@
         <v>1429</v>
       </c>
       <c r="B1431" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="C1431" t="s">
         <v>9</v>
@@ -33560,7 +33606,7 @@
         <v>1430</v>
       </c>
       <c r="B1432" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="C1432" t="s">
         <v>14</v>
@@ -33580,7 +33626,7 @@
         <v>1431</v>
       </c>
       <c r="B1433" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="C1433" t="s">
         <v>9</v>
@@ -33600,7 +33646,7 @@
         <v>1432</v>
       </c>
       <c r="B1434" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C1434" t="s">
         <v>14</v>
@@ -33620,7 +33666,7 @@
         <v>1433</v>
       </c>
       <c r="B1435" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="C1435" t="s">
         <v>24</v>
@@ -33640,7 +33686,7 @@
         <v>1434</v>
       </c>
       <c r="B1436" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C1436" t="s">
         <v>9</v>
@@ -33660,7 +33706,7 @@
         <v>1435</v>
       </c>
       <c r="B1437" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="C1437" t="s">
         <v>14</v>
@@ -33680,7 +33726,7 @@
         <v>1436</v>
       </c>
       <c r="B1438" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="C1438" t="s">
         <v>6</v>
@@ -33700,7 +33746,7 @@
         <v>1437</v>
       </c>
       <c r="B1439" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="C1439" t="s">
         <v>6</v>
@@ -33720,7 +33766,7 @@
         <v>1438</v>
       </c>
       <c r="B1440" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="C1440" t="s">
         <v>9</v>
@@ -33740,7 +33786,7 @@
         <v>1439</v>
       </c>
       <c r="B1441" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="C1441" t="s">
         <v>38</v>
@@ -33760,7 +33806,7 @@
         <v>1440</v>
       </c>
       <c r="B1442" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="C1442" t="s">
         <v>9</v>
@@ -33780,7 +33826,7 @@
         <v>1441</v>
       </c>
       <c r="B1443" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="C1443" t="s">
         <v>9</v>
@@ -33800,7 +33846,7 @@
         <v>1442</v>
       </c>
       <c r="B1444" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="C1444" t="s">
         <v>9</v>
@@ -33820,7 +33866,7 @@
         <v>1443</v>
       </c>
       <c r="B1445" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="C1445" t="s">
         <v>9</v>
@@ -33840,7 +33886,7 @@
         <v>1444</v>
       </c>
       <c r="B1446" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="C1446" t="s">
         <v>9</v>
@@ -33860,7 +33906,7 @@
         <v>1445</v>
       </c>
       <c r="B1447" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="C1447" t="s">
         <v>14</v>
@@ -33880,7 +33926,7 @@
         <v>1446</v>
       </c>
       <c r="B1448" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="C1448" t="s">
         <v>38</v>
@@ -33900,7 +33946,7 @@
         <v>1447</v>
       </c>
       <c r="B1449" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="C1449" t="s">
         <v>14</v>
@@ -33920,7 +33966,7 @@
         <v>1448</v>
       </c>
       <c r="B1450" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="C1450" t="s">
         <v>9</v>
@@ -33940,7 +33986,7 @@
         <v>1449</v>
       </c>
       <c r="B1451" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="C1451" t="s">
         <v>46</v>
@@ -33960,7 +34006,7 @@
         <v>1450</v>
       </c>
       <c r="B1452" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="C1452" t="s">
         <v>64</v>
@@ -33980,7 +34026,7 @@
         <v>1451</v>
       </c>
       <c r="B1453" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="C1453" t="s">
         <v>9</v>
@@ -34000,7 +34046,7 @@
         <v>1452</v>
       </c>
       <c r="B1454" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="C1454" t="s">
         <v>9</v>
@@ -34020,7 +34066,7 @@
         <v>1453</v>
       </c>
       <c r="B1455" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="C1455" t="s">
         <v>14</v>
@@ -34040,7 +34086,7 @@
         <v>1454</v>
       </c>
       <c r="B1456" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="C1456" t="s">
         <v>9</v>
@@ -34060,7 +34106,7 @@
         <v>1455</v>
       </c>
       <c r="B1457" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="C1457" t="s">
         <v>9</v>
@@ -34080,7 +34126,7 @@
         <v>1456</v>
       </c>
       <c r="B1458" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="C1458" t="s">
         <v>9</v>
@@ -34100,7 +34146,7 @@
         <v>1457</v>
       </c>
       <c r="B1459" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="C1459" t="s">
         <v>14</v>
@@ -34120,7 +34166,7 @@
         <v>1458</v>
       </c>
       <c r="B1460" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="C1460" t="s">
         <v>14</v>
@@ -34140,7 +34186,7 @@
         <v>1459</v>
       </c>
       <c r="B1461" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C1461" t="s">
         <v>14</v>
@@ -34160,7 +34206,7 @@
         <v>1460</v>
       </c>
       <c r="B1462" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C1462" t="s">
         <v>77</v>
@@ -34180,7 +34226,7 @@
         <v>1461</v>
       </c>
       <c r="B1463" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="C1463" t="s">
         <v>77</v>
@@ -34200,7 +34246,7 @@
         <v>1462</v>
       </c>
       <c r="B1464" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="C1464" t="s">
         <v>9</v>
@@ -34220,7 +34266,7 @@
         <v>1463</v>
       </c>
       <c r="B1465" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="C1465" t="s">
         <v>38</v>
@@ -34240,7 +34286,7 @@
         <v>1464</v>
       </c>
       <c r="B1466" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="C1466" t="s">
         <v>9</v>
@@ -34260,7 +34306,7 @@
         <v>1465</v>
       </c>
       <c r="B1467" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="C1467" t="s">
         <v>14</v>
@@ -34280,7 +34326,7 @@
         <v>1466</v>
       </c>
       <c r="B1468" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="C1468" t="s">
         <v>77</v>
@@ -34300,7 +34346,7 @@
         <v>1467</v>
       </c>
       <c r="B1469" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="C1469" t="s">
         <v>9</v>
@@ -34320,7 +34366,7 @@
         <v>1468</v>
       </c>
       <c r="B1470" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="C1470" t="s">
         <v>9</v>
@@ -34340,7 +34386,7 @@
         <v>1469</v>
       </c>
       <c r="B1471" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="C1471" t="s">
         <v>38</v>
@@ -34360,7 +34406,7 @@
         <v>1470</v>
       </c>
       <c r="B1472" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="C1472" t="s">
         <v>14</v>
@@ -34380,7 +34426,7 @@
         <v>1471</v>
       </c>
       <c r="B1473" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="C1473" t="s">
         <v>14</v>
@@ -34400,7 +34446,7 @@
         <v>1472</v>
       </c>
       <c r="B1474" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="C1474" t="s">
         <v>14</v>
@@ -34420,7 +34466,7 @@
         <v>1473</v>
       </c>
       <c r="B1475" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="C1475" t="s">
         <v>20</v>
@@ -34440,7 +34486,7 @@
         <v>1474</v>
       </c>
       <c r="B1476" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="C1476" t="s">
         <v>38</v>
@@ -34460,7 +34506,7 @@
         <v>1475</v>
       </c>
       <c r="B1477" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C1477" t="s">
         <v>20</v>
@@ -34480,7 +34526,7 @@
         <v>1476</v>
       </c>
       <c r="B1478" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="C1478" t="s">
         <v>24</v>
@@ -34500,7 +34546,7 @@
         <v>1477</v>
       </c>
       <c r="B1479" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="C1479" t="s">
         <v>9</v>
@@ -34520,7 +34566,7 @@
         <v>1478</v>
       </c>
       <c r="B1480" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="C1480" t="s">
         <v>20</v>
@@ -34540,7 +34586,7 @@
         <v>1479</v>
       </c>
       <c r="B1481" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="C1481" t="s">
         <v>9</v>
@@ -34560,7 +34606,7 @@
         <v>1480</v>
       </c>
       <c r="B1482" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C1482" t="s">
         <v>14</v>
@@ -34580,7 +34626,7 @@
         <v>1481</v>
       </c>
       <c r="B1483" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C1483" t="s">
         <v>77</v>
@@ -34600,7 +34646,7 @@
         <v>1482</v>
       </c>
       <c r="B1484" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C1484" t="s">
         <v>14</v>
@@ -34620,7 +34666,7 @@
         <v>1483</v>
       </c>
       <c r="B1485" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C1485" t="s">
         <v>14</v>
@@ -34640,7 +34686,7 @@
         <v>1484</v>
       </c>
       <c r="B1486" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C1486" t="s">
         <v>14</v>
@@ -34660,7 +34706,7 @@
         <v>1485</v>
       </c>
       <c r="B1487" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C1487" t="s">
         <v>46</v>
@@ -34680,7 +34726,7 @@
         <v>1486</v>
       </c>
       <c r="B1488" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C1488" t="s">
         <v>6</v>
@@ -34700,7 +34746,7 @@
         <v>1487</v>
       </c>
       <c r="B1489" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C1489" t="s">
         <v>14</v>
@@ -34720,7 +34766,7 @@
         <v>1488</v>
       </c>
       <c r="B1490" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="C1490" t="s">
         <v>24</v>
@@ -34740,7 +34786,7 @@
         <v>1489</v>
       </c>
       <c r="B1491" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C1491" t="s">
         <v>68</v>
@@ -34760,7 +34806,7 @@
         <v>1490</v>
       </c>
       <c r="B1492" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C1492" t="s">
         <v>9</v>
@@ -34780,7 +34826,7 @@
         <v>1491</v>
       </c>
       <c r="B1493" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C1493" t="s">
         <v>6</v>
@@ -34800,7 +34846,7 @@
         <v>1492</v>
       </c>
       <c r="B1494" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="C1494" t="s">
         <v>64</v>
@@ -34820,7 +34866,7 @@
         <v>1493</v>
       </c>
       <c r="B1495" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="C1495" t="s">
         <v>6</v>
@@ -34840,7 +34886,7 @@
         <v>1494</v>
       </c>
       <c r="B1496" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C1496" t="s">
         <v>9</v>
@@ -34860,7 +34906,7 @@
         <v>1495</v>
       </c>
       <c r="B1497" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="C1497" t="s">
         <v>38</v>
@@ -34880,7 +34926,7 @@
         <v>1496</v>
       </c>
       <c r="B1498" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="C1498" t="s">
         <v>14</v>
@@ -34893,6 +34939,226 @@
       </c>
       <c r="F1498">
         <v>8.0202903822174392</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1499" s="1">
+        <v>1497</v>
+      </c>
+      <c r="B1499" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C1499" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1499" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1499">
+        <v>49.526040000000002</v>
+      </c>
+      <c r="F1499">
+        <v>5.9035700000000002</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1500" s="1">
+        <v>1498</v>
+      </c>
+      <c r="B1500" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C1500" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1500" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1500">
+        <v>47.312370000000001</v>
+      </c>
+      <c r="F1500">
+        <v>9.59192</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1501" s="1">
+        <v>1499</v>
+      </c>
+      <c r="B1501" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C1501" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1501" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1501">
+        <v>47.198889999999999</v>
+      </c>
+      <c r="F1501">
+        <v>9.6696299999999997</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1502" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B1502" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C1502" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1502" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1502">
+        <v>50.393729999999998</v>
+      </c>
+      <c r="F1502">
+        <v>4.3716600000000003</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1503" s="1">
+        <v>1501</v>
+      </c>
+      <c r="B1503" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C1503" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1503" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1503">
+        <v>49.541049999999998</v>
+      </c>
+      <c r="F1503">
+        <v>5.7599</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1504" s="1">
+        <v>1502</v>
+      </c>
+      <c r="B1504" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C1504" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D1504" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1504">
+        <v>49.567239999999998</v>
+      </c>
+      <c r="F1504">
+        <v>5.9399199999999999</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1505" s="1">
+        <v>1503</v>
+      </c>
+      <c r="B1505" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C1505" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D1505" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1505">
+        <v>49.510260000000002</v>
+      </c>
+      <c r="F1505">
+        <v>5.9476699999999996</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1506" s="1">
+        <v>1504</v>
+      </c>
+      <c r="B1506" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C1506" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1506" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1506">
+        <v>47.236310000000003</v>
+      </c>
+      <c r="F1506">
+        <v>11.39242</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1507" s="1">
+        <v>1505</v>
+      </c>
+      <c r="B1507" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C1507" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1507" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1507">
+        <v>47.753050000000002</v>
+      </c>
+      <c r="F1507">
+        <v>10.31691</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1508" s="1">
+        <v>1506</v>
+      </c>
+      <c r="B1508" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C1508" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1508" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1508">
+        <v>47.189259999999997</v>
+      </c>
+      <c r="F1508">
+        <v>9.7197300000000002</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1509" s="1">
+        <v>1507</v>
+      </c>
+      <c r="B1509" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C1509" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1509" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1509">
+        <v>49.310519999999997</v>
+      </c>
+      <c r="F1509">
+        <v>22.54757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>